<commit_message>
modified excel and txt file
</commit_message>
<xml_diff>
--- a/ObjectOrientedProgramming/SchoolManagement/students.xlsx
+++ b/ObjectOrientedProgramming/SchoolManagement/students.xlsx
@@ -29,67 +29,67 @@
     <t>A</t>
   </si>
   <si>
-    <t xml:space="preserve"> "james"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abcd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "lyndsay"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "adffr@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "han"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abcrgrgd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "yolo"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abvfdvefcd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "matt"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abcwrfrd@abcd"</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t xml:space="preserve"> "harvey"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "ar33bcd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "harry"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abc4t34gd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "chloe"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abcgssrgrd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "linda"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abgrgikrcd@abcd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "duncan"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "abjumnycd@abcd"</t>
+    <t xml:space="preserve"> james</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lyndsay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> han</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> harvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> harry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chloe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> linda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> duncan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abcd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adffr@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abcrgrgd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abvfdvefcd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abcwrfrd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ar33bcd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abc4t34gd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abcgssrgrd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abgrgikrcd@abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abjumnycd@abcd</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,13 +423,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F1">
         <v>89</v>
@@ -449,7 +449,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>91</v>
@@ -463,13 +463,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>45</v>
@@ -483,13 +483,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>32</v>
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>75</v>
@@ -517,19 +517,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>77</v>
@@ -537,19 +537,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>65</v>
@@ -557,19 +557,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>92</v>
@@ -577,19 +577,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>57</v>
@@ -597,13 +597,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>12</v>

</xml_diff>